<commit_message>
[revision] made docs as decode happens in 2nd cycle
</commit_message>
<xml_diff>
--- a/Project-v1/Documents/2-operand/NO_haza_no_forw_WRONG/no_haza_no_forw_WRONG_2_OP.xlsx
+++ b/Project-v1/Documents/2-operand/NO_haza_no_forw_WRONG/no_haza_no_forw_WRONG_2_OP.xlsx
@@ -57,9 +57,6 @@
     <t>Iadd R3,R5,2</t>
   </si>
   <si>
-    <t xml:space="preserve">R3 = 0  </t>
-  </si>
-  <si>
     <t>R1 = 5</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>R4 = F320</t>
   </si>
   <si>
-    <t>R5 = 2</t>
-  </si>
-  <si>
     <t>Add R1,R4,R4</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>R4 = F325</t>
   </si>
   <si>
-    <t>R6 = FFFF 0CE0</t>
-  </si>
-  <si>
     <t>AND  R7,R6,R6</t>
   </si>
   <si>
@@ -123,21 +114,9 @@
     <t xml:space="preserve">SWAP R2,R5 </t>
   </si>
   <si>
-    <t>R2=2  R5=64</t>
-  </si>
-  <si>
-    <t>R2 = 64 , R5 =2</t>
-  </si>
-  <si>
     <t>ADD  R5,R2,R2</t>
   </si>
   <si>
-    <t>R5 =2 , R2 = 64</t>
-  </si>
-  <si>
-    <t>R2 = 66</t>
-  </si>
-  <si>
     <t>Data Inconsistency</t>
   </si>
   <si>
@@ -151,6 +130,27 @@
   </si>
   <si>
     <t>SHR R2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3 = FFFD  </t>
+  </si>
+  <si>
+    <t>R5 = FFFF</t>
+  </si>
+  <si>
+    <t>R2 = 64 , R5 = FFFF</t>
+  </si>
+  <si>
+    <t>R5 = FFFF , R2 = 64</t>
+  </si>
+  <si>
+    <t>R2 = 10063</t>
+  </si>
+  <si>
+    <t>R2=FFFF R5=64</t>
+  </si>
+  <si>
+    <t>R6 = FFFF0CE0</t>
   </si>
 </sst>
 </file>
@@ -210,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -229,6 +229,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,7 +537,7 @@
   <dimension ref="A1:AQ21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA26" sqref="AA26"/>
+      <selection activeCell="AI21" sqref="AI21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +583,7 @@
         <v>5</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P2" s="8"/>
       <c r="Q2" s="8"/>
@@ -609,7 +613,7 @@
         <v>5</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="R3" s="8"/>
       <c r="S3" s="8"/>
@@ -632,11 +636,11 @@
       <c r="L4" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="M4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="S4" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="T4" s="8"/>
       <c r="U4" s="8"/>
@@ -664,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="T5" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="U5" s="8"/>
       <c r="V5" s="8"/>
@@ -673,19 +677,19 @@
     </row>
     <row r="6" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
       <c r="K6" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="4" t="s">
         <v>2</v>
       </c>
       <c r="M6" t="s">
@@ -701,7 +705,7 @@
         <v>5</v>
       </c>
       <c r="W6" s="8" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
@@ -710,12 +714,12 @@
     </row>
     <row r="7" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -738,7 +742,7 @@
         <v>5</v>
       </c>
       <c r="X7" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
@@ -747,12 +751,12 @@
     </row>
     <row r="8" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
@@ -775,7 +779,7 @@
         <v>5</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="AA8" s="8"/>
       <c r="AB8" s="8"/>
@@ -785,12 +789,12 @@
     </row>
     <row r="9" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="7" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -813,7 +817,7 @@
         <v>5</v>
       </c>
       <c r="AB9" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="AC9" s="8"/>
       <c r="AD9" s="8"/>
@@ -823,12 +827,12 @@
     </row>
     <row r="10" spans="1:43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
@@ -851,7 +855,7 @@
         <v>5</v>
       </c>
       <c r="AD10" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="AE10" s="8"/>
       <c r="AF10" s="8"/>
@@ -861,12 +865,12 @@
     </row>
     <row r="11" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -892,7 +896,7 @@
         <v>5</v>
       </c>
       <c r="AF11" s="8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AG11" s="8"/>
       <c r="AH11" s="8"/>
@@ -902,12 +906,12 @@
     </row>
     <row r="12" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -920,10 +924,10 @@
       <c r="S12" t="s">
         <v>1</v>
       </c>
-      <c r="T12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U12" t="s">
+      <c r="T12" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="U12" s="11" t="s">
         <v>2</v>
       </c>
       <c r="V12" t="s">
@@ -936,7 +940,7 @@
         <v>5</v>
       </c>
       <c r="AH12" s="8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AI12" s="8"/>
       <c r="AJ12" s="8"/>
@@ -946,12 +950,12 @@
     </row>
     <row r="13" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -980,7 +984,7 @@
         <v>5</v>
       </c>
       <c r="AJ13" s="8" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="AK13" s="8"/>
       <c r="AL13" s="8"/>
@@ -990,12 +994,12 @@
     </row>
     <row r="14" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6"/>
       <c r="D14" s="7" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1024,7 +1028,7 @@
         <v>5</v>
       </c>
       <c r="AL14" s="8" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AM14" s="8"/>
       <c r="AN14" s="8"/>
@@ -1035,7 +1039,7 @@
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
@@ -1043,7 +1047,7 @@
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="3"/>
       <c r="D20" s="6" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
@@ -1051,18 +1055,38 @@
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="5"/>
       <c r="D21" s="6" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="T5:X5"/>
+    <mergeCell ref="W6:AA6"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="X7:AB7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="Z8:AE8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="AB9:AG9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="AD10:AI10"/>
     <mergeCell ref="AJ13:AO13"/>
     <mergeCell ref="D14:F14"/>
     <mergeCell ref="A14:C14"/>
@@ -1073,31 +1097,11 @@
     <mergeCell ref="D12:F12"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="AH12:AM12"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="AB9:AG9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="AD10:AI10"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="X7:AB7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="Z8:AE8"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="Q3:S3"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="T5:X5"/>
-    <mergeCell ref="W6:AA6"/>
-    <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>